<commit_message>
test with server end
</commit_message>
<xml_diff>
--- a/server communication REST standard.xlsx
+++ b/server communication REST standard.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
   <si>
     <t>Route</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -105,6 +105,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>ownerID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>title</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -126,6 +130,70 @@
   </si>
   <si>
     <t>photoURL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>owner</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>,…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">user </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{ id }</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{ pollID }</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>item</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{ }</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/polls</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>title</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>totalVotes (default = 0)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>startTime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>maxVotesForSingleItem (default = 1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>state (default = "EDITING")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/polls/:pollID</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -185,18 +253,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="9">
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -525,20 +605,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="3" max="3" width="21.83203125" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+    <col min="3" max="5" width="21.83203125" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -548,11 +629,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -562,16 +643,16 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:8">
       <c r="C3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -581,101 +662,222 @@
       <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:8">
       <c r="C6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
         <v>14</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="E9" t="s">
+    <row r="9" spans="1:8">
+      <c r="G9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="E10" t="s">
+    <row r="10" spans="1:8">
+      <c r="G10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="E11" t="s">
+    <row r="11" spans="1:8">
+      <c r="G11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="H12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="H13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="H14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="G15" t="s">
         <v>24</v>
       </c>
-      <c r="F11" t="s">
+      <c r="H15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="F12" t="s">
+    <row r="16" spans="1:8">
+      <c r="H16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="H17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="G18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="H19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="H20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="H21" t="s">
+        <v>28</v>
+      </c>
+      <c r="I21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="I22" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
-      <c r="F13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="F14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="E15" t="s">
+    <row r="23" spans="1:9">
+      <c r="I23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="H24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="G25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="G26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="G27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="C29" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="C30" t="s">
         <v>18</v>
       </c>
-      <c r="F15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="F16" t="s">
+      <c r="D30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="C31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F33" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="5:6">
-      <c r="F17" t="s">
+    <row r="34" spans="1:6">
+      <c r="C34" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="5:6">
-      <c r="F18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="5:6">
-      <c r="E19" t="s">
-        <v>23</v>
-      </c>
-      <c r="F19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="5:6">
-      <c r="F20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="5:6">
-      <c r="F21" t="s">
-        <v>22</v>
+      <c r="F34" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="C35" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="C36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="C37" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="C38" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>